<commit_message>
Update all tests for new format for Study sheet
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/address.xlsx
+++ b/tests/integration_test_files/address.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D89B8F-20C3-A846-AB08-817179018036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC2B7D4-583D-7248-BC25-A4D2EE245F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35040" yWindow="3820" windowWidth="33260" windowHeight="19480" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="35040" yWindow="3820" windowWidth="33260" windowHeight="19480" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="291">
   <si>
     <t>Epoch</t>
   </si>
@@ -499,12 +499,6 @@
     <t>protocolVersion</t>
   </si>
   <si>
-    <t>protocolAmendment</t>
-  </si>
-  <si>
-    <t>protocolEffectiveDate</t>
-  </si>
-  <si>
     <t>protocolStatus</t>
   </si>
   <si>
@@ -517,18 +511,12 @@
     <t>Something Public</t>
   </si>
   <si>
-    <t>Somethign Clever</t>
-  </si>
-  <si>
     <t>draft</t>
   </si>
   <si>
     <t>Somethign Clever But New</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>businessTherapeuticAreas</t>
   </si>
   <si>
@@ -929,6 +917,12 @@
   </si>
   <si>
     <t>EU12345</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>ADDRESS1</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1007,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1051,9 +1045,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1069,28 +1060,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1407,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1423,218 +1411,172 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B6" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+    </row>
+    <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B7" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="B10" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="B11" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="B12" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="B13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="G9" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="B14" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="15">
-        <v>40179</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G11" s="15">
-        <v>40544</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
@@ -2173,29 +2115,29 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C5" t="s">
         <v>134</v>
       </c>
       <c r="D5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F5" t="s">
         <v>112</v>
@@ -2204,7 +2146,7 @@
         <v>118</v>
       </c>
       <c r="H5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2235,63 +2177,63 @@
       <c r="A1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>189</v>
+      <c r="B1" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="C3" t="s">
-        <v>257</v>
-      </c>
-      <c r="D3" t="s">
-        <v>259</v>
-      </c>
-      <c r="E3" t="s">
-        <v>194</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>195</v>
-      </c>
       <c r="G3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2323,138 +2265,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="G1" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="H1" s="22" t="s">
         <v>200</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>210</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>211</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2480,105 +2422,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>227</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>204</v>
+      <c r="B1" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2602,18 +2544,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2625,7 +2567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9227F54-17C1-E44A-AD70-49AE8CBF35F9}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -2639,22 +2581,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="21" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2669,13 +2611,13 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2689,30 +2631,30 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
         <v>54</v>
       </c>
       <c r="F3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="D4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>291</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="D4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2736,107 +2678,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>252</v>
+      <c r="A1" s="16" t="s">
+        <v>248</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>253</v>
+      <c r="A2" s="16" t="s">
+        <v>249</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="B3" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="B4" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="B5" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>48</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
       <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>178</v>
+      <c r="A9" s="16" t="s">
+        <v>174</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>179</v>
+      <c r="A10" s="16" t="s">
+        <v>175</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
@@ -2844,8 +2786,8 @@
       <c r="E10" s="25"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
-        <v>225</v>
+      <c r="A12" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>43</v>
@@ -2865,16 +2807,16 @@
         <v>41</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2882,16 +2824,16 @@
         <v>42</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2908,16 +2850,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2941,20 +2883,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>273</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>274</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2962,16 +2904,16 @@
         <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2982,13 +2924,13 @@
         <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3015,14 +2957,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>262</v>
+      <c r="A1" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3030,10 +2972,10 @@
         <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3041,10 +2983,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3052,10 +2994,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3063,10 +3005,10 @@
         <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3095,13 +3037,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>180</v>
+      <c r="A1" s="16" t="s">
+        <v>176</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="C1" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -3119,13 +3061,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="A2" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -3145,13 +3087,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>184</v>
+      <c r="A3" s="16" t="s">
+        <v>180</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C3" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -3173,7 +3115,7 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -3195,7 +3137,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -3217,7 +3159,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -3239,30 +3181,30 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="17" t="s">
-        <v>222</v>
+      <c r="C7" s="16" t="s">
+        <v>218</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
-      <c r="C8" s="17" t="s">
-        <v>223</v>
+      <c r="C8" s="16" t="s">
+        <v>219</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
@@ -3276,14 +3218,14 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="24" t="s">
-        <v>224</v>
+      <c r="C9" s="22" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3365,17 +3307,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>281</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>283</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>284</v>
+      <c r="A1" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3383,7 +3325,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3391,13 +3333,13 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update to Objective and Endpoints
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/address.xlsx
+++ b/tests/integration_test_files/address.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC2B7D4-583D-7248-BC25-A4D2EE245F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A25822-49C9-F942-9564-3FA9896E7AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35040" yWindow="3820" windowWidth="33260" windowHeight="19480" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="34740" yWindow="7780" windowWidth="42040" windowHeight="19480" activeTab="9" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="295">
   <si>
     <t>Epoch</t>
   </si>
@@ -316,9 +316,6 @@
     <t>endpointDescription</t>
   </si>
   <si>
-    <t>endpointPurposeDescription</t>
-  </si>
-  <si>
     <t>endpointLevel</t>
   </si>
   <si>
@@ -923,6 +920,21 @@
   </si>
   <si>
     <t>ADDRESS1</t>
+  </si>
+  <si>
+    <t>objectiveLabel</t>
+  </si>
+  <si>
+    <t>objectiveText</t>
+  </si>
+  <si>
+    <t>endpointLabel</t>
+  </si>
+  <si>
+    <t>endpointText</t>
+  </si>
+  <si>
+    <t>endpointPurpose</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1028,9 +1040,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1071,10 +1080,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1395,7 +1404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1411,11 +1420,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>289</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>290</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -1423,10 +1432,10 @@
       <c r="H1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>40</v>
       </c>
       <c r="E2"/>
@@ -1435,10 +1444,10 @@
       <c r="H2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E3"/>
@@ -1447,10 +1456,10 @@
       <c r="H3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>57</v>
       </c>
       <c r="E4"/>
@@ -1459,10 +1468,10 @@
       <c r="H4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E5"/>
@@ -1471,11 +1480,11 @@
       <c r="H5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>142</v>
+      <c r="A6" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
@@ -1483,11 +1492,11 @@
       <c r="H6"/>
     </row>
     <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>143</v>
+      <c r="A7" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>142</v>
       </c>
       <c r="E7"/>
       <c r="F7"/>
@@ -1495,11 +1504,11 @@
       <c r="H7"/>
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>155</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>156</v>
       </c>
       <c r="E8"/>
       <c r="F8"/>
@@ -1507,11 +1516,11 @@
       <c r="H8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>150</v>
+      <c r="A9" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>149</v>
       </c>
       <c r="E9"/>
       <c r="F9"/>
@@ -1519,11 +1528,11 @@
       <c r="H9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>151</v>
+      <c r="A10" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>150</v>
       </c>
       <c r="E10"/>
       <c r="F10"/>
@@ -1531,11 +1540,11 @@
       <c r="H10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>152</v>
+      <c r="A11" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="E11"/>
       <c r="F11"/>
@@ -1543,11 +1552,11 @@
       <c r="H11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>154</v>
+      <c r="A12" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>153</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
@@ -1555,10 +1564,10 @@
       <c r="H12"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E13"/>
@@ -1567,11 +1576,11 @@
       <c r="H13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
-        <v>149</v>
+      <c r="A14" s="18" t="s">
+        <v>148</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -1579,50 +1588,50 @@
       <c r="H14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1635,407 +1644,564 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="44" customWidth="1"/>
-    <col min="3" max="4" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="59.5" customWidth="1"/>
-    <col min="6" max="7" width="31.5" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="49" customWidth="1"/>
+    <col min="5" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="70.5" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="G1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" s="9" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="E2" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="K3" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
+      <c r="J4" s="9"/>
+      <c r="K4" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="J5" s="9"/>
+      <c r="K5" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10" t="s">
+      <c r="J6" s="9"/>
+      <c r="K6" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
+      <c r="J7" s="9"/>
+      <c r="K7" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
+      <c r="J8" s="9"/>
+      <c r="K8" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
+      <c r="J9" s="9"/>
+      <c r="K9" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10" t="s">
+      <c r="J10" s="9"/>
+      <c r="K10" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
+      <c r="J11" s="9"/>
+      <c r="K11" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10" t="s">
+      <c r="J12" s="9"/>
+      <c r="K12" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="J13" s="9"/>
+      <c r="K13" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2062,91 +2228,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>130</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
         <v>133</v>
       </c>
-      <c r="B2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>134</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" t="s">
         <v>135</v>
-      </c>
-      <c r="E2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" t="s">
         <v>166</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" t="s">
         <v>167</v>
       </c>
-      <c r="C5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>168</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" t="s">
         <v>169</v>
-      </c>
-      <c r="F5" t="s">
-        <v>112</v>
-      </c>
-      <c r="G5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H5" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2175,65 +2341,65 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="16" t="s">
         <v>184</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
         <v>186</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2" t="s">
         <v>187</v>
-      </c>
-      <c r="C2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E3" t="s">
         <v>189</v>
       </c>
-      <c r="B3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" t="s">
-        <v>253</v>
-      </c>
-      <c r="D3" t="s">
-        <v>255</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" t="s">
         <v>191</v>
-      </c>
-      <c r="G3" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2265,138 +2431,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>199</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>206</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2422,105 +2588,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>199</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>231</v>
-      </c>
       <c r="D5" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2544,18 +2710,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
         <v>161</v>
-      </c>
-      <c r="B2" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2581,22 +2747,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2611,13 +2777,13 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2631,30 +2797,30 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E3" t="s">
         <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="C4" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="D4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>287</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>286</v>
-      </c>
-      <c r="D4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2678,116 +2844,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>247</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>246</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="B3" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
-        <v>221</v>
+      <c r="A12" s="15" t="s">
+        <v>220</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>43</v>
@@ -2807,16 +2973,16 @@
         <v>41</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>226</v>
-      </c>
       <c r="D13" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2824,16 +2990,16 @@
         <v>42</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>226</v>
-      </c>
       <c r="D14" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2850,16 +3016,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2883,20 +3049,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>270</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2904,16 +3070,16 @@
         <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2924,17 +3090,17 @@
         <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>275</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E4" s="11"/>
+      <c r="E4" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2957,14 +3123,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>257</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2972,10 +3138,10 @@
         <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2983,10 +3149,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2994,10 +3160,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3005,10 +3171,10 @@
         <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3037,13 +3203,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -3052,22 +3218,22 @@
       <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="28"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -3087,13 +3253,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -3113,9 +3279,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="16" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="15" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -3135,9 +3301,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="16" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -3157,9 +3323,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="16" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -3179,32 +3345,32 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="16" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="15" t="s">
         <v>218</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="16" t="s">
-        <v>219</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
@@ -3218,14 +3384,14 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>220</v>
+      <c r="C9" s="21" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3307,17 +3473,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>279</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3325,7 +3491,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3333,13 +3499,13 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" t="s">
         <v>282</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3367,7 +3533,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>59</v>
@@ -3381,7 +3547,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
         <v>60</v>
@@ -3395,7 +3561,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
         <v>61</v>
@@ -3409,7 +3575,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
         <v>60</v>
@@ -3423,7 +3589,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Fix issue with old spreadsheets
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/address.xlsx
+++ b/tests/integration_test_files/address.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BD7D7C-F52F-284A-A710-BFB0EAFC7C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F341CE61-BE51-5945-AF48-2EB0D353B4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34740" yWindow="7780" windowWidth="42040" windowHeight="19480" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="34740" yWindow="7780" windowWidth="42040" windowHeight="19480" activeTab="9" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="297">
   <si>
     <t>Epoch</t>
   </si>
@@ -935,6 +935,12 @@
   </si>
   <si>
     <t>Somewhere,In a District,In a City,In a big state,12345,FRA</t>
+  </si>
+  <si>
+    <t>objectiveDictionary</t>
+  </si>
+  <si>
+    <t>endpointDictionary</t>
   </si>
 </sst>
 </file>
@@ -1080,10 +1086,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1644,10 +1650,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:G14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1656,15 +1662,16 @@
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="49" customWidth="1"/>
-    <col min="5" max="6" width="18.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.5" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="70.5" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" customWidth="1"/>
-    <col min="11" max="11" width="22.83203125" customWidth="1"/>
+    <col min="5" max="7" width="18.83203125" customWidth="1"/>
+    <col min="8" max="8" width="20.5" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="70.5" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" customWidth="1"/>
+    <col min="12" max="12" width="22.83203125" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>112</v>
       </c>
@@ -1681,25 +1688,31 @@
         <v>86</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="M1" s="21" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>114</v>
       </c>
@@ -1711,19 +1724,20 @@
       <c r="E2" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="9"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>115</v>
       </c>
@@ -1735,199 +1749,210 @@
       <c r="E3" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G3" s="9"/>
       <c r="H3" s="9"/>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="9"/>
+      <c r="G4" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="9"/>
+      <c r="J4" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="9"/>
+      <c r="L4" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G5" s="9"/>
       <c r="H5" s="9"/>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="9"/>
+      <c r="J5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="9"/>
+      <c r="L5" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="G6" s="9"/>
       <c r="H6" s="9"/>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="9"/>
+      <c r="J6" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="9"/>
+      <c r="L6" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="9"/>
+      <c r="G7" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="9"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="9"/>
+      <c r="J7" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="9"/>
+      <c r="L7" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G8" s="9"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="9"/>
+      <c r="J8" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="9"/>
+      <c r="L8" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="G9" s="9"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="9"/>
+      <c r="J9" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="9"/>
+      <c r="L9" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="G10" s="9"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="9"/>
+      <c r="J10" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="9"/>
+      <c r="L10" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G11" s="9"/>
       <c r="H11" s="9"/>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="9"/>
+      <c r="J11" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="9"/>
+      <c r="G12" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="G12" s="9"/>
       <c r="H12" s="9"/>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="9"/>
+      <c r="J12" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="G13" s="9"/>
       <c r="H13" s="9"/>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="9"/>
+      <c r="J13" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="9"/>
+      <c r="L13" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -1938,8 +1963,9 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1950,8 +1976,9 @@
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1962,8 +1989,9 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1974,8 +2002,9 @@
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -1986,8 +2015,9 @@
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1998,8 +2028,9 @@
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -2010,8 +2041,9 @@
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -2022,8 +2054,9 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -2034,8 +2067,9 @@
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2046,8 +2080,9 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -2058,8 +2093,9 @@
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -2070,8 +2106,9 @@
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L25" s="9"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -2082,8 +2119,9 @@
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L26" s="9"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -2094,8 +2132,9 @@
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L27" s="9"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -2106,8 +2145,9 @@
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L28" s="9"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -2118,8 +2158,9 @@
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L29" s="9"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -2130,8 +2171,9 @@
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L30" s="9"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -2142,8 +2184,9 @@
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -2154,8 +2197,9 @@
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L32" s="9"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -2166,8 +2210,9 @@
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L33" s="9"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -2178,8 +2223,9 @@
       <c r="I34" s="9"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L34" s="9"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -2190,8 +2236,9 @@
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L35" s="9"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -2202,6 +2249,7 @@
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2733,7 +2781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9227F54-17C1-E44A-AD70-49AE8CBF35F9}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2869,34 +2917,34 @@
       <c r="A3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
@@ -3016,16 +3064,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update test file results
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/address.xlsx
+++ b/tests/integration_test_files/address.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F114A7-FB4F-C745-9D52-9EE6B95E8459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AEFB6D-4883-DC4C-AAA9-CEF985E1F833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49580" yWindow="5920" windowWidth="42040" windowHeight="19480" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="49580" yWindow="5920" windowWidth="42040" windowHeight="19480" activeTab="8" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="359">
   <si>
     <t>Screening</t>
   </si>
@@ -900,18 +900,12 @@
     <t>SPONSOR: A=B</t>
   </si>
   <si>
-    <t>M11: role1=role1</t>
-  </si>
-  <si>
     <t>DRUG</t>
   </si>
   <si>
     <t>FDA: A=B</t>
   </si>
   <si>
-    <t xml:space="preserve"> M11: desig1=desig_1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1 Day</t>
   </si>
   <si>
@@ -948,12 +942,6 @@
     <t xml:space="preserve"> Int Label 2</t>
   </si>
   <si>
-    <t>M11: role2=role2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> M11: desig2=desig_2</t>
-  </si>
-  <si>
     <t>Admin 2</t>
   </si>
   <si>
@@ -1132,6 +1120,15 @@
   </si>
   <si>
     <t>encounter</t>
+  </si>
+  <si>
+    <t>Experimental Intervention</t>
+  </si>
+  <si>
+    <t>IMP</t>
+  </si>
+  <si>
+    <t>NIMP (AxMP)</t>
   </si>
 </sst>
 </file>
@@ -1285,10 +1282,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1308,9 +1305,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1348,7 +1345,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1454,7 +1451,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1596,7 +1593,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1878,10 +1875,10 @@
         <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>49</v>
@@ -1892,10 +1889,10 @@
         <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>50</v>
@@ -1927,7 +1924,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>253</v>
@@ -1939,13 +1936,13 @@
         <v>264</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="H1" s="19" t="s">
         <v>52</v>
@@ -1953,10 +1950,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -1970,24 +1967,24 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="G3" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B4" t="s">
+        <v>311</v>
+      </c>
+      <c r="G4" t="s">
         <v>313</v>
-      </c>
-      <c r="B4" t="s">
-        <v>315</v>
-      </c>
-      <c r="G4" t="s">
-        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3264,34 +3261,34 @@
       <c r="A3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
@@ -3411,16 +3408,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3581,7 +3578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
@@ -3608,19 +3605,19 @@
         <v>253</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -3637,13 +3634,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>196</v>
@@ -3660,7 +3657,7 @@
         <v>264</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -3669,7 +3666,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>196</v>
@@ -3681,46 +3678,46 @@
         <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
       <c r="C5" s="15" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>349</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="15"/>
       <c r="C6" s="15" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -3732,7 +3729,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="15" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
@@ -3754,7 +3751,7 @@
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="15" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>181</v>
@@ -3871,123 +3868,123 @@
         <v>46</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>319</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G2" t="s">
+        <v>325</v>
+      </c>
+      <c r="H2" t="s">
         <v>326</v>
-      </c>
-      <c r="E2" t="s">
-        <v>327</v>
-      </c>
-      <c r="F2" t="s">
-        <v>328</v>
-      </c>
-      <c r="G2" t="s">
-        <v>329</v>
-      </c>
-      <c r="H2" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="I3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4" t="s">
+        <v>333</v>
+      </c>
+      <c r="C4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D4" t="s">
+        <v>335</v>
+      </c>
+      <c r="E4" t="s">
+        <v>330</v>
+      </c>
+      <c r="F4" t="s">
+        <v>330</v>
+      </c>
+      <c r="G4" t="s">
         <v>336</v>
-      </c>
-      <c r="B4" t="s">
-        <v>337</v>
-      </c>
-      <c r="C4" t="s">
-        <v>338</v>
-      </c>
-      <c r="D4" t="s">
-        <v>339</v>
-      </c>
-      <c r="E4" t="s">
-        <v>334</v>
-      </c>
-      <c r="F4" t="s">
-        <v>334</v>
-      </c>
-      <c r="G4" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C5" t="s">
+        <v>339</v>
+      </c>
+      <c r="D5" t="s">
+        <v>340</v>
+      </c>
+      <c r="E5" t="s">
         <v>341</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F5" t="s">
+        <v>330</v>
+      </c>
+      <c r="G5" t="s">
         <v>342</v>
       </c>
-      <c r="C5" t="s">
-        <v>343</v>
-      </c>
-      <c r="D5" t="s">
-        <v>344</v>
-      </c>
-      <c r="E5" t="s">
-        <v>345</v>
-      </c>
-      <c r="F5" t="s">
-        <v>334</v>
-      </c>
-      <c r="G5" t="s">
-        <v>346</v>
-      </c>
       <c r="H5" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="I5" t="s">
         <v>7</v>
@@ -3995,31 +3992,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B6" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C6" t="s">
         <v>196</v>
       </c>
       <c r="D6" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E6" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G6" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="H6" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -4093,8 +4090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34FEBA59-8EC5-C345-AC55-D637FAA20B65}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4103,7 +4100,7 @@
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="24.5" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" customWidth="1"/>
     <col min="7" max="7" width="23.5" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
@@ -4194,49 +4191,49 @@
         <v>281</v>
       </c>
       <c r="E2" t="s">
+        <v>356</v>
+      </c>
+      <c r="F2" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="G2" t="s">
         <v>283</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>357</v>
+      </c>
+      <c r="I2" t="s">
         <v>284</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>285</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>286</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>287</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>288</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>289</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>290</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>291</v>
-      </c>
-      <c r="O2" t="s">
-        <v>292</v>
-      </c>
-      <c r="P2" t="s">
-        <v>293</v>
       </c>
       <c r="Q2" t="s">
         <v>159</v>
       </c>
       <c r="R2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="S2" s="25" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -4244,58 +4241,58 @@
         <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D3" t="s">
         <v>281</v>
       </c>
       <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="G3" t="s">
+        <v>283</v>
+      </c>
+      <c r="H3" t="s">
+        <v>358</v>
+      </c>
+      <c r="I3" t="s">
+        <v>284</v>
+      </c>
+      <c r="J3" t="s">
+        <v>296</v>
+      </c>
+      <c r="K3" t="s">
+        <v>297</v>
+      </c>
+      <c r="L3" t="s">
         <v>298</v>
       </c>
-      <c r="F3" s="24" t="s">
-        <v>283</v>
-      </c>
-      <c r="G3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="M3" t="s">
+        <v>288</v>
+      </c>
+      <c r="N3" t="s">
+        <v>289</v>
+      </c>
+      <c r="O3" t="s">
+        <v>290</v>
+      </c>
+      <c r="P3" t="s">
         <v>299</v>
-      </c>
-      <c r="I3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J3" t="s">
-        <v>300</v>
-      </c>
-      <c r="K3" t="s">
-        <v>301</v>
-      </c>
-      <c r="L3" t="s">
-        <v>302</v>
-      </c>
-      <c r="M3" t="s">
-        <v>290</v>
-      </c>
-      <c r="N3" t="s">
-        <v>291</v>
-      </c>
-      <c r="O3" t="s">
-        <v>292</v>
-      </c>
-      <c r="P3" t="s">
-        <v>303</v>
       </c>
       <c r="Q3" t="s">
         <v>159</v>
       </c>
       <c r="R3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="S3" s="25" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for objective level CT
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/address.xlsx
+++ b/tests/integration_test_files/address.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AEFB6D-4883-DC4C-AAA9-CEF985E1F833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FEC377-4289-1744-BFFE-B2451003E253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49580" yWindow="5920" windowWidth="42040" windowHeight="19480" activeTab="8" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="49580" yWindow="5920" windowWidth="42040" windowHeight="19480" activeTab="11" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -231,9 +231,6 @@
     <t>The primary efficacy objective for this study is to evaluate the efficacy of TCZ compared with placebo in combination with SOC for the treatment of severe COVID-19 pneumonia</t>
   </si>
   <si>
-    <t>Study Primary Objective</t>
-  </si>
-  <si>
     <t>Clinical status assessed using a 7-category ordinal scale at Day 28</t>
   </si>
   <si>
@@ -243,9 +240,6 @@
     <t>The secondary efficacy objective for this study is to evaluate the efficacy of TCZ compared with placebo in combination with SOC for the treatment of severe COVID-19 pneumonia</t>
   </si>
   <si>
-    <t>Study Secondary Objective</t>
-  </si>
-  <si>
     <t>Time to clinical improvement (TTCI) defined as a National Early Warning Score 2 (NEWS2) of &lt;=2 maintained for 24 hours</t>
   </si>
   <si>
@@ -1129,6 +1123,12 @@
   </si>
   <si>
     <t>NIMP (AxMP)</t>
+  </si>
+  <si>
+    <t>Primary Objective</t>
+  </si>
+  <si>
+    <t>Secondary Objective</t>
   </si>
 </sst>
 </file>
@@ -1282,10 +1282,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1305,9 +1305,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1345,7 +1345,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1451,7 +1451,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1593,7 +1593,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1620,10 +1620,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -1680,10 +1680,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>110</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
@@ -1692,10 +1692,10 @@
     </row>
     <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>109</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>111</v>
       </c>
       <c r="E7"/>
       <c r="F7"/>
@@ -1704,10 +1704,10 @@
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E8"/>
       <c r="F8"/>
@@ -1716,10 +1716,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E9"/>
       <c r="F9"/>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E10"/>
       <c r="F10"/>
@@ -1740,10 +1740,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E11"/>
       <c r="F11"/>
@@ -1752,10 +1752,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>17</v>
@@ -1776,10 +1776,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -1858,13 +1858,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>47</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>48</v>
@@ -1872,13 +1872,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>49</v>
@@ -1886,13 +1886,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>50</v>
@@ -1924,25 +1924,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>47</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H1" s="19" t="s">
         <v>52</v>
@@ -1950,10 +1950,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -1967,24 +1967,24 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G3" t="s">
         <v>310</v>
-      </c>
-      <c r="G3" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B4" t="s">
         <v>309</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" t="s">
         <v>311</v>
-      </c>
-      <c r="G4" t="s">
-        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -1996,8 +1996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2017,48 +2017,48 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>54</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>55</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>56</v>
       </c>
       <c r="I1" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="K1" s="21" t="s">
         <v>257</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>258</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>259</v>
       </c>
       <c r="L1" s="21" t="s">
         <v>57</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2066,44 +2066,44 @@
         <v>58</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>59</v>
+        <v>357</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>63</v>
+        <v>358</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -2113,16 +2113,16 @@
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -2132,16 +2132,16 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -2151,16 +2151,16 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -2170,16 +2170,16 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -2189,16 +2189,16 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -2208,16 +2208,16 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -2227,16 +2227,16 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -2246,16 +2246,16 @@
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -2265,16 +2265,16 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -2284,16 +2284,16 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -2621,90 +2621,90 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>100</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>105</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" t="s">
         <v>102</v>
-      </c>
-      <c r="D2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
         <v>134</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>135</v>
       </c>
-      <c r="C5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" t="s">
         <v>136</v>
-      </c>
-      <c r="E5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G5" t="s">
-        <v>86</v>
-      </c>
-      <c r="H5" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2733,65 +2733,65 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="E1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>151</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E2" t="s">
         <v>154</v>
-      </c>
-      <c r="B2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" t="s">
-        <v>218</v>
-      </c>
-      <c r="D2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>158</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="G3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2824,137 +2824,137 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>166</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="E5" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2981,104 +2981,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>200</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>196</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -3102,18 +3102,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
         <v>129</v>
-      </c>
-      <c r="B1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3169,13 +3169,13 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -3189,30 +3189,30 @@
         <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E3" t="s">
         <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="D4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>250</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>250</v>
-      </c>
-      <c r="D4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -3237,10 +3237,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
@@ -3248,10 +3248,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -3261,41 +3261,41 @@
       <c r="A3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="B3" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="B4" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="B5" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
@@ -3306,7 +3306,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C7" s="26"/>
       <c r="D7" s="26"/>
@@ -3317,7 +3317,7 @@
         <v>36</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
@@ -3325,10 +3325,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
@@ -3336,7 +3336,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -3345,7 +3345,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>30</v>
@@ -3365,16 +3365,16 @@
         <v>28</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>192</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -3382,16 +3382,16 @@
         <v>29</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>192</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -3408,16 +3408,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3442,19 +3442,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>235</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>236</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -3462,16 +3462,16 @@
         <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -3482,13 +3482,13 @@
         <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3516,13 +3516,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>222</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3530,10 +3530,10 @@
         <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3541,10 +3541,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3552,10 +3552,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3563,10 +3563,10 @@
         <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3596,36 +3596,36 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>47</v>
@@ -3634,30 +3634,30 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -3666,10 +3666,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -3678,46 +3678,46 @@
         <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
       <c r="C5" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="15"/>
       <c r="C6" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -3729,7 +3729,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
@@ -3751,22 +3751,22 @@
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="15" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -3777,7 +3777,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3856,135 +3856,135 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>317</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="E2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F2" t="s">
         <v>322</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>323</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>324</v>
-      </c>
-      <c r="G2" t="s">
-        <v>325</v>
-      </c>
-      <c r="H2" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C3" t="s">
         <v>327</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E3" t="s">
+        <v>322</v>
+      </c>
+      <c r="F3" t="s">
         <v>328</v>
-      </c>
-      <c r="C3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D3" t="s">
-        <v>322</v>
-      </c>
-      <c r="E3" t="s">
-        <v>324</v>
-      </c>
-      <c r="F3" t="s">
-        <v>330</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C4" t="s">
         <v>332</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>333</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
+        <v>328</v>
+      </c>
+      <c r="F4" t="s">
+        <v>328</v>
+      </c>
+      <c r="G4" t="s">
         <v>334</v>
-      </c>
-      <c r="D4" t="s">
-        <v>335</v>
-      </c>
-      <c r="E4" t="s">
-        <v>330</v>
-      </c>
-      <c r="F4" t="s">
-        <v>330</v>
-      </c>
-      <c r="G4" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C5" t="s">
         <v>337</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>338</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>339</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
+        <v>328</v>
+      </c>
+      <c r="G5" t="s">
         <v>340</v>
       </c>
-      <c r="E5" t="s">
-        <v>341</v>
-      </c>
-      <c r="F5" t="s">
-        <v>330</v>
-      </c>
-      <c r="G5" t="s">
-        <v>342</v>
-      </c>
       <c r="H5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I5" t="s">
         <v>7</v>
@@ -3992,31 +3992,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>341</v>
+      </c>
+      <c r="B6" t="s">
+        <v>342</v>
+      </c>
+      <c r="C6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" t="s">
+        <v>338</v>
+      </c>
+      <c r="E6" t="s">
         <v>343</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
+        <v>328</v>
+      </c>
+      <c r="G6" t="s">
         <v>344</v>
       </c>
-      <c r="C6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D6" t="s">
-        <v>340</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
+        <v>324</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>345</v>
-      </c>
-      <c r="F6" t="s">
-        <v>330</v>
-      </c>
-      <c r="G6" t="s">
-        <v>346</v>
-      </c>
-      <c r="H6" t="s">
-        <v>326</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -4043,16 +4043,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>244</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>245</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4060,7 +4060,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4068,13 +4068,13 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4090,7 +4090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34FEBA59-8EC5-C345-AC55-D637FAA20B65}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -4120,179 +4120,179 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>47</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>46</v>
       </c>
       <c r="G1" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="Q1" s="21" t="s">
         <v>274</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>275</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="S1" s="21" t="s">
         <v>276</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>277</v>
-      </c>
-      <c r="S1" s="21" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D2" t="s">
         <v>279</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>354</v>
+      </c>
+      <c r="F2" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>281</v>
       </c>
-      <c r="E2" t="s">
-        <v>356</v>
-      </c>
-      <c r="F2" s="24" t="s">
+      <c r="H2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I2" t="s">
         <v>282</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>283</v>
       </c>
-      <c r="H2" t="s">
-        <v>357</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>284</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>285</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>286</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>287</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>288</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>289</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
+        <v>157</v>
+      </c>
+      <c r="R2" t="s">
         <v>290</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" s="25" t="s">
         <v>291</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>159</v>
-      </c>
-      <c r="R2" t="s">
-        <v>292</v>
-      </c>
-      <c r="S2" s="25" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="G3" t="s">
+        <v>281</v>
+      </c>
+      <c r="H3" t="s">
+        <v>356</v>
+      </c>
+      <c r="I3" t="s">
         <v>282</v>
       </c>
-      <c r="G3" t="s">
-        <v>283</v>
-      </c>
-      <c r="H3" t="s">
-        <v>358</v>
-      </c>
-      <c r="I3" t="s">
-        <v>284</v>
-      </c>
       <c r="J3" t="s">
+        <v>294</v>
+      </c>
+      <c r="K3" t="s">
+        <v>295</v>
+      </c>
+      <c r="L3" t="s">
         <v>296</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
+        <v>286</v>
+      </c>
+      <c r="N3" t="s">
+        <v>287</v>
+      </c>
+      <c r="O3" t="s">
+        <v>288</v>
+      </c>
+      <c r="P3" t="s">
         <v>297</v>
       </c>
-      <c r="L3" t="s">
-        <v>298</v>
-      </c>
-      <c r="M3" t="s">
-        <v>288</v>
-      </c>
-      <c r="N3" t="s">
-        <v>289</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
+        <v>157</v>
+      </c>
+      <c r="R3" t="s">
         <v>290</v>
       </c>
-      <c r="P3" t="s">
-        <v>299</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>159</v>
-      </c>
-      <c r="R3" t="s">
-        <v>292</v>
-      </c>
       <c r="S3" s="25" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to XL sheets for timelines
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/address.xlsx
+++ b/tests/integration_test_files/address.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FEC377-4289-1744-BFFE-B2451003E253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1531AAF5-38DA-C246-9983-31C0D3C1E2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49580" yWindow="5920" windowWidth="42040" windowHeight="19480" activeTab="11" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="49580" yWindow="5920" windowWidth="42040" windowHeight="19480" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="359">
   <si>
     <t>Screening</t>
   </si>
@@ -1282,10 +1282,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1996,7 +1996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
@@ -3261,34 +3261,34 @@
       <c r="A3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
@@ -3408,16 +3408,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3582,7 +3582,7 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" sqref="A1:H1048576"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3781,9 +3781,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
@@ -3807,9 +3805,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
@@ -3842,7 +3838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7496F0CE-4BE5-5143-8535-0A433E9A5B8A}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Bug and test fix
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/address.xlsx
+++ b/tests/integration_test_files/address.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973B3B01-09BC-8C4C-8E98-FE56A1456659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEBEFCD-8E05-144C-8160-2DEC2FFB28F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49580" yWindow="5920" windowWidth="42040" windowHeight="19480" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="55640" yWindow="7620" windowWidth="42040" windowHeight="19480" firstSheet="2" activeTab="12" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="366">
   <si>
     <t>Screening</t>
   </si>
@@ -1141,13 +1141,22 @@
   </si>
   <si>
     <t>line1, line2, schipol, Amsterdam, North, 12345, NLD</t>
+  </si>
+  <si>
+    <t>populationSubset</t>
+  </si>
+  <si>
+    <t>intercurrentEventText</t>
+  </si>
+  <si>
+    <t>ICE Text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1173,14 +1182,6 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1231,7 +1232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1259,10 +1260,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1286,9 +1283,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1631,7 +1628,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>249</v>
       </c>
       <c r="B1" s="10" t="s">
@@ -1643,7 +1640,7 @@
       <c r="H1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -1655,10 +1652,10 @@
       <c r="H2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E3"/>
@@ -1667,7 +1664,7 @@
       <c r="H3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -1679,7 +1676,7 @@
       <c r="H4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -1691,7 +1688,7 @@
       <c r="H5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="16" t="s">
         <v>104</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1703,7 +1700,7 @@
       <c r="H6"/>
     </row>
     <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>105</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -1715,10 +1712,10 @@
       <c r="H7"/>
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>120</v>
       </c>
       <c r="E8"/>
@@ -1727,7 +1724,7 @@
       <c r="H8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="16" t="s">
         <v>108</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -1739,7 +1736,7 @@
       <c r="H9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="16" t="s">
         <v>109</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -1751,7 +1748,7 @@
       <c r="H10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="16" t="s">
         <v>110</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -1763,7 +1760,7 @@
       <c r="H11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="16" t="s">
         <v>111</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -1775,10 +1772,10 @@
       <c r="H12"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E13"/>
@@ -1787,7 +1784,7 @@
       <c r="H13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="16" t="s">
         <v>113</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1869,16 +1866,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1920,7 +1917,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1935,28 +1932,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>300</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="17" t="s">
         <v>302</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="17" t="s">
         <v>310</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2009,7 +2006,7 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2028,43 +2025,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="19" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2615,49 +2612,56 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="61.83203125" customWidth="1"/>
+    <col min="3" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" customWidth="1"/>
+    <col min="7" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="61.83203125" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="19" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J1" s="19" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -2668,32 +2672,46 @@
         <v>98</v>
       </c>
       <c r="D2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E2" t="s">
         <v>99</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>103</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>74</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>81</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H3" t="s">
+      <c r="J2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D3" s="10"/>
+      <c r="I3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H4" t="s">
+      <c r="J3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D4" s="10"/>
+      <c r="I4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -2704,19 +2722,25 @@
         <v>98</v>
       </c>
       <c r="D5" t="s">
+        <v>307</v>
+      </c>
+      <c r="E5" t="s">
         <v>132</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>133</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>76</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>82</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>134</v>
+      </c>
+      <c r="J5" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -2747,22 +2771,22 @@
       <c r="A1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2835,28 +2859,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2992,19 +3016,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3137,7 +3161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9227F54-17C1-E44A-AD70-49AE8CBF35F9}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3151,22 +3175,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="18" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3211,22 +3235,22 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>246</v>
       </c>
       <c r="D4" t="s">
         <v>136</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="20" t="s">
         <v>362</v>
       </c>
     </row>
@@ -3268,115 +3292,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="13" t="s">
         <v>183</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -3473,19 +3497,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3547,13 +3571,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>220</v>
       </c>
     </row>
@@ -3627,13 +3651,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>140</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>249</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -3653,13 +3677,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -3679,13 +3703,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>144</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="13" t="s">
         <v>260</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -3705,8 +3729,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="C4" s="15" t="s">
+      <c r="A4" s="13"/>
+      <c r="C4" s="13" t="s">
         <v>44</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -3726,8 +3750,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="C5" s="15" t="s">
+      <c r="A5" s="13"/>
+      <c r="C5" s="13" t="s">
         <v>347</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -3747,8 +3771,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="C6" s="15" t="s">
+      <c r="A6" s="13"/>
+      <c r="C6" s="13" t="s">
         <v>349</v>
       </c>
       <c r="D6" s="2"/>
@@ -3760,7 +3784,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>350</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -3782,7 +3806,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>351</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -3802,13 +3826,13 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="19" t="s">
         <v>182</v>
       </c>
     </row>
@@ -4070,16 +4094,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4147,61 +4171,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="19" t="s">
         <v>274</v>
       </c>
     </row>
@@ -4221,7 +4245,7 @@
       <c r="E2" t="s">
         <v>352</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="22" t="s">
         <v>278</v>
       </c>
       <c r="G2" t="s">
@@ -4260,7 +4284,7 @@
       <c r="R2" t="s">
         <v>288</v>
       </c>
-      <c r="S2" s="25" t="s">
+      <c r="S2" s="23" t="s">
         <v>289</v>
       </c>
     </row>
@@ -4280,7 +4304,7 @@
       <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="22" t="s">
         <v>278</v>
       </c>
       <c r="G3" t="s">
@@ -4319,7 +4343,7 @@
       <c r="R3" t="s">
         <v>288</v>
       </c>
-      <c r="S3" s="25" t="s">
+      <c r="S3" s="23" t="s">
         <v>289</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated XL test files
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/address.xlsx
+++ b/tests/integration_test_files/address.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/github/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AC0A77-F0D4-7641-B62A-FB8E8715A9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28CA5CD-B786-AC4C-AF15-BE78D8569C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="500" windowWidth="50160" windowHeight="27240" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" firstSheet="1" activeTab="12" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -1114,12 +1114,6 @@
     <t>NIMP (AxMP)</t>
   </si>
   <si>
-    <t>Primary Objective</t>
-  </si>
-  <si>
-    <t>Secondary Objective</t>
-  </si>
-  <si>
     <t>ACME Pharma US</t>
   </si>
   <si>
@@ -1166,6 +1160,12 @@
   </si>
   <si>
     <t>interventional</t>
+  </si>
+  <si>
+    <t>Trial Primary Objective</t>
+  </si>
+  <si>
+    <t>Trial Secondary Objective</t>
   </si>
 </sst>
 </file>
@@ -1307,10 +1307,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1628,7 +1628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:B5"/>
     </sheetView>
   </sheetViews>
@@ -2235,8 +2235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2305,7 +2305,7 @@
         <v>55</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>353</v>
+        <v>369</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9" t="s">
@@ -2330,7 +2330,7 @@
         <v>58</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>354</v>
+        <v>370</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9" t="s">
@@ -2870,7 +2870,7 @@
         <v>48</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>93</v>
@@ -2888,7 +2888,7 @@
         <v>94</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2920,7 +2920,7 @@
         <v>99</v>
       </c>
       <c r="J2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -2929,7 +2929,7 @@
         <v>126</v>
       </c>
       <c r="J3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -2938,7 +2938,7 @@
         <v>127</v>
       </c>
       <c r="J4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2970,7 +2970,7 @@
         <v>132</v>
       </c>
       <c r="J5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -3451,10 +3451,10 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E3" t="s">
         <v>133</v>
@@ -3480,7 +3480,7 @@
         <v>134</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -3488,13 +3488,13 @@
         <v>37</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E5" t="s">
         <v>133</v>
@@ -3521,7 +3521,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>22</v>
@@ -3537,10 +3537,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3553,10 +3553,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B5" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -3605,34 +3605,34 @@
       <c r="A3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -3647,7 +3647,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>122</v>
@@ -3661,7 +3661,7 @@
         <v>36</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -3692,7 +3692,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
@@ -3703,7 +3703,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
@@ -3774,18 +3774,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update integration test files
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/address.xlsx
+++ b/tests/integration_test_files/address.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/github/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28CA5CD-B786-AC4C-AF15-BE78D8569C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47364F8D-664F-8446-9EB8-69704E5D3CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" firstSheet="1" activeTab="12" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" firstSheet="1" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -454,12 +454,6 @@
     <t>Really really bad shit</t>
   </si>
   <si>
-    <t>Clinical Study Sponsor</t>
-  </si>
-  <si>
-    <t>Study Registry</t>
-  </si>
-  <si>
     <t>SPONSOR:T2_DIABETES=Type 2 diabetes, SNOMED: 73211009=Diabetes mellitus (disorder)</t>
   </si>
   <si>
@@ -1166,6 +1160,12 @@
   </si>
   <si>
     <t>Trial Secondary Objective</t>
+  </si>
+  <si>
+    <t>Pharmaceutical Company</t>
+  </si>
+  <si>
+    <t>Clinical Study Registry</t>
   </si>
 </sst>
 </file>
@@ -1645,10 +1645,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -1900,61 +1900,61 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>44</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="G1" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="J1" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="K1" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="N1" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="O1" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="P1" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="R1" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>270</v>
-      </c>
-      <c r="R1" s="19" t="s">
-        <v>271</v>
-      </c>
-      <c r="S1" s="19" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -1962,58 +1962,58 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D2" t="s">
         <v>273</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>348</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>275</v>
       </c>
-      <c r="E2" t="s">
-        <v>350</v>
-      </c>
-      <c r="F2" s="22" t="s">
+      <c r="H2" t="s">
+        <v>349</v>
+      </c>
+      <c r="I2" t="s">
         <v>276</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>277</v>
       </c>
-      <c r="H2" t="s">
-        <v>351</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>278</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>279</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>280</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>281</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>282</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>283</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
+        <v>151</v>
+      </c>
+      <c r="R2" t="s">
         <v>284</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" s="23" t="s">
         <v>285</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>153</v>
-      </c>
-      <c r="R2" t="s">
-        <v>286</v>
-      </c>
-      <c r="S2" s="23" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -2021,58 +2021,58 @@
         <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="G3" t="s">
+        <v>275</v>
+      </c>
+      <c r="H3" t="s">
+        <v>350</v>
+      </c>
+      <c r="I3" t="s">
         <v>276</v>
       </c>
-      <c r="G3" t="s">
-        <v>277</v>
-      </c>
-      <c r="H3" t="s">
-        <v>352</v>
-      </c>
-      <c r="I3" t="s">
-        <v>278</v>
-      </c>
       <c r="J3" t="s">
+        <v>288</v>
+      </c>
+      <c r="K3" t="s">
+        <v>289</v>
+      </c>
+      <c r="L3" t="s">
         <v>290</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
+        <v>280</v>
+      </c>
+      <c r="N3" t="s">
+        <v>281</v>
+      </c>
+      <c r="O3" t="s">
+        <v>282</v>
+      </c>
+      <c r="P3" t="s">
         <v>291</v>
       </c>
-      <c r="L3" t="s">
-        <v>292</v>
-      </c>
-      <c r="M3" t="s">
-        <v>282</v>
-      </c>
-      <c r="N3" t="s">
-        <v>283</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R3" t="s">
         <v>284</v>
       </c>
-      <c r="P3" t="s">
-        <v>293</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>153</v>
-      </c>
-      <c r="R3" t="s">
-        <v>286</v>
-      </c>
       <c r="S3" s="23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2097,13 +2097,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>44</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>45</v>
@@ -2114,10 +2114,10 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>46</v>
@@ -2128,10 +2128,10 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>47</v>
@@ -2163,25 +2163,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>44</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H1" s="17" t="s">
         <v>49</v>
@@ -2189,10 +2189,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -2206,24 +2206,24 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G3" t="s">
         <v>304</v>
-      </c>
-      <c r="G3" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B4" t="s">
         <v>303</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" t="s">
         <v>305</v>
-      </c>
-      <c r="G4" t="s">
-        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -2235,7 +2235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -2262,16 +2262,16 @@
         <v>51</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>52</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>77</v>
@@ -2280,19 +2280,19 @@
         <v>53</v>
       </c>
       <c r="I1" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>251</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>252</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>253</v>
       </c>
       <c r="L1" s="19" t="s">
         <v>54</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -2305,7 +2305,7 @@
         <v>55</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9" t="s">
@@ -2330,7 +2330,7 @@
         <v>58</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9" t="s">
@@ -2870,7 +2870,7 @@
         <v>48</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>93</v>
@@ -2888,7 +2888,7 @@
         <v>94</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2902,7 +2902,7 @@
         <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E2" t="s">
         <v>98</v>
@@ -2920,7 +2920,7 @@
         <v>99</v>
       </c>
       <c r="J2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -2929,7 +2929,7 @@
         <v>126</v>
       </c>
       <c r="J3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -2938,7 +2938,7 @@
         <v>127</v>
       </c>
       <c r="J4" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2952,7 +2952,7 @@
         <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E5" t="s">
         <v>130</v>
@@ -2970,7 +2970,7 @@
         <v>132</v>
       </c>
       <c r="J5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -3002,62 +3002,62 @@
         <v>71</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>145</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" t="s">
         <v>148</v>
-      </c>
-      <c r="B2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D3" t="s">
-        <v>215</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>152</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="G3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3093,134 +3093,134 @@
         <v>71</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>160</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="E5" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3250,101 +3250,101 @@
         <v>71</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>194</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>195</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3391,8 +3391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B20DF789-F467-8042-B95F-EAD3364F9C51}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3414,7 +3414,7 @@
         <v>20</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>21</v>
@@ -3437,10 +3437,10 @@
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>134</v>
+        <v>370</v>
       </c>
       <c r="F2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -3451,36 +3451,36 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E3" t="s">
-        <v>133</v>
+        <v>369</v>
       </c>
       <c r="F3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>370</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -3488,16 +3488,16 @@
         <v>37</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3521,7 +3521,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>22</v>
@@ -3537,26 +3537,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>244</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3581,10 +3581,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -3592,10 +3592,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -3606,7 +3606,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
@@ -3617,7 +3617,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
@@ -3647,7 +3647,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>122</v>
@@ -3661,7 +3661,7 @@
         <v>36</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -3669,10 +3669,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
@@ -3680,7 +3680,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
@@ -3692,7 +3692,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
@@ -3703,7 +3703,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
@@ -3711,7 +3711,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>30</v>
@@ -3731,16 +3731,16 @@
         <v>28</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -3748,16 +3748,16 @@
         <v>29</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C16" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -3774,6 +3774,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B4:E4"/>
@@ -3781,11 +3786,6 @@
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3810,19 +3810,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>229</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -3830,16 +3830,16 @@
         <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -3850,13 +3850,13 @@
         <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3884,13 +3884,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>216</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3898,10 +3898,10 @@
         <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3909,10 +3909,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3920,10 +3920,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3931,10 +3931,10 @@
         <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -3964,36 +3964,36 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>44</v>
@@ -4002,30 +4002,30 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -4034,10 +4034,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -4046,46 +4046,46 @@
         <v>43</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="C5" s="13" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -4097,7 +4097,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
@@ -4119,22 +4119,22 @@
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="13" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -4145,7 +4145,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -4220,135 +4220,135 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>311</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="E2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F2" t="s">
         <v>316</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>317</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>318</v>
-      </c>
-      <c r="G2" t="s">
-        <v>319</v>
-      </c>
-      <c r="H2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C3" t="s">
         <v>321</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E3" t="s">
+        <v>316</v>
+      </c>
+      <c r="F3" t="s">
         <v>322</v>
-      </c>
-      <c r="C3" t="s">
-        <v>323</v>
-      </c>
-      <c r="D3" t="s">
-        <v>316</v>
-      </c>
-      <c r="E3" t="s">
-        <v>318</v>
-      </c>
-      <c r="F3" t="s">
-        <v>324</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C4" t="s">
         <v>326</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>327</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F4" t="s">
+        <v>322</v>
+      </c>
+      <c r="G4" t="s">
         <v>328</v>
-      </c>
-      <c r="D4" t="s">
-        <v>329</v>
-      </c>
-      <c r="E4" t="s">
-        <v>324</v>
-      </c>
-      <c r="F4" t="s">
-        <v>324</v>
-      </c>
-      <c r="G4" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B5" t="s">
+        <v>330</v>
+      </c>
+      <c r="C5" t="s">
         <v>331</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>332</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>333</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
+        <v>322</v>
+      </c>
+      <c r="G5" t="s">
         <v>334</v>
       </c>
-      <c r="E5" t="s">
-        <v>335</v>
-      </c>
-      <c r="F5" t="s">
-        <v>324</v>
-      </c>
-      <c r="G5" t="s">
-        <v>336</v>
-      </c>
       <c r="H5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I5" t="s">
         <v>7</v>
@@ -4356,31 +4356,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>335</v>
+      </c>
+      <c r="B6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" t="s">
+        <v>332</v>
+      </c>
+      <c r="E6" t="s">
         <v>337</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G6" t="s">
         <v>338</v>
       </c>
-      <c r="C6" t="s">
-        <v>190</v>
-      </c>
-      <c r="D6" t="s">
-        <v>334</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
+        <v>318</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>339</v>
-      </c>
-      <c r="F6" t="s">
-        <v>324</v>
-      </c>
-      <c r="G6" t="s">
-        <v>340</v>
-      </c>
-      <c r="H6" t="s">
-        <v>320</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -4407,16 +4407,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>238</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4424,7 +4424,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4432,13 +4432,13 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>